<commit_message>
New examples, new make_heatmap argument, improve shiny UI
</commit_message>
<xml_diff>
--- a/inst/extdata/waffle_input_example.xlsx
+++ b/inst/extdata/waffle_input_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\My Drive\R projects\viztools\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B956B866-B977-4BB8-9136-E04928EBC7CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D125DEA1-DA82-4495-A84B-9B47C06BA1E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2325" yWindow="1200" windowWidth="26745" windowHeight="13890" xr2:uid="{DA3DE0FC-772D-4B6B-A37E-292E19C523AC}"/>
+    <workbookView xWindow="1395" yWindow="1005" windowWidth="26745" windowHeight="13890" xr2:uid="{DA3DE0FC-772D-4B6B-A37E-292E19C523AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>fraction</t>
   </si>
@@ -42,6 +42,12 @@
   </si>
   <si>
     <t>Membrane</t>
+  </si>
+  <si>
+    <t>Periplasm</t>
+  </si>
+  <si>
+    <t>Unannotated</t>
   </si>
 </sst>
 </file>
@@ -393,18 +399,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08D325FC-EF8F-4309-A34A-08CE9892320A}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="2" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -414,8 +422,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -425,8 +439,14 @@
       <c r="C2">
         <v>5</v>
       </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -436,8 +456,14 @@
       <c r="C3">
         <v>10</v>
       </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -447,8 +473,14 @@
       <c r="C4">
         <v>15</v>
       </c>
+      <c r="D4">
+        <v>25</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -456,6 +488,46 @@
         <v>20</v>
       </c>
       <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>40</v>
+      </c>
+      <c r="C6">
+        <v>30</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>60</v>
+      </c>
+      <c r="C7">
+        <v>35</v>
+      </c>
+      <c r="D7">
+        <v>15</v>
+      </c>
+      <c r="E7">
         <v>10</v>
       </c>
     </row>
@@ -465,6 +537,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005D5DBE6C31380A43B0F8DF017AFDB3C2" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5593feddfd3a1af1bd36e6f0c66ba0f0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="05f87325a7941fe022abeebe778951f9">
     <xsd:element name="properties">
@@ -578,22 +665,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD7714FA-157D-4312-A55C-A141C0822F6F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E8E0B40-FF42-4998-96D8-AF2FE2B05BF6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79DD4086-1757-427E-892B-5C908F483B19}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -607,27 +702,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E8E0B40-FF42-4998-96D8-AF2FE2B05BF6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD7714FA-157D-4312-A55C-A141C0822F6F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>